<commit_message>
Actualizacoes dia 27 as 17
</commit_message>
<xml_diff>
--- a/comunidaderesumo.xlsx
+++ b/comunidaderesumo.xlsx
@@ -13,15 +13,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Regiao</t>
   </si>
   <si>
+    <t>CHIMANIMANI</t>
+  </si>
+  <si>
     <t>GORONGOSA</t>
   </si>
   <si>
     <t>nome_comunidade</t>
+  </si>
+  <si>
+    <t>MUSSAPA</t>
+  </si>
+  <si>
+    <t>MPUNGA</t>
   </si>
   <si>
     <t>NHAMU E NHADINDE</t>
@@ -86,7 +95,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -94,25 +103,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
@@ -120,25 +129,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0">
         <v>1</v>
       </c>
       <c r="D2" s="0">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="E2" s="0">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="F2" s="0">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="G2" s="0">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="H2" s="0">
-        <v>64</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3">
@@ -146,25 +155,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="0">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E3" s="0">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="F3" s="0">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G3" s="0">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="H3" s="0">
-        <v>78</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4">
@@ -172,24 +181,102 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0">
+        <v>2</v>
+      </c>
+      <c r="D4" s="0">
+        <v>18</v>
+      </c>
+      <c r="E4" s="0">
+        <v>12</v>
+      </c>
+      <c r="F4" s="0">
+        <v>32</v>
+      </c>
+      <c r="G4" s="0">
+        <v>8</v>
+      </c>
+      <c r="H4" s="0">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0">
+        <v>26</v>
+      </c>
+      <c r="E5" s="0">
+        <v>17</v>
+      </c>
+      <c r="F5" s="0">
+        <v>15</v>
+      </c>
+      <c r="G5" s="0">
+        <v>6</v>
+      </c>
+      <c r="H5" s="0">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0">
+        <v>2</v>
+      </c>
+      <c r="D6" s="0">
+        <v>30</v>
+      </c>
+      <c r="E6" s="0">
+        <v>32</v>
+      </c>
+      <c r="F6" s="0">
+        <v>9</v>
+      </c>
+      <c r="G6" s="0">
+        <v>7</v>
+      </c>
+      <c r="H6" s="0">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0">
         <v>3</v>
       </c>
-      <c r="C4" s="0">
-        <v>3</v>
-      </c>
-      <c r="D4" s="0">
+      <c r="D7" s="0">
         <v>38</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E7" s="0">
         <v>35</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F7" s="0">
         <v>8</v>
       </c>
-      <c r="G4" s="0">
-        <v>6</v>
-      </c>
-      <c r="H4" s="0">
+      <c r="G7" s="0">
+        <v>6</v>
+      </c>
+      <c r="H7" s="0">
         <v>87</v>
       </c>
     </row>

</xml_diff>